<commit_message>
Write tests that fail for read_csv() and read_excel()
</commit_message>
<xml_diff>
--- a/pdtable/test/io/input/foo.xlsx
+++ b/pdtable/test/io/input/foo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeaco\repos\pdtable\pdtable\test\readers\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeaco\repos\pdtable\pdtable\test\io\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01B0DF2-1B41-41B9-9615-99C6570B924A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1221CD82-89E3-42F8-AFFA-77B254447387}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0C2B564F-1ED4-41D9-860E-6D5D2FB64FA7}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>all</t>
   </si>
@@ -112,6 +112,21 @@
   </si>
   <si>
     <t>Crime and Punishment</t>
+  </si>
+  <si>
+    <t>diameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cm</t>
+  </si>
+  <si>
+    <t>melting_point</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> K</t>
+  </si>
+  <si>
+    <t>**this_one_is_transposed*</t>
   </si>
 </sst>
 </file>
@@ -463,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B433973-3070-4A41-BCCD-AE6DD659FC75}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -578,17 +593,17 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -596,7 +611,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -604,7 +619,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
@@ -612,7 +627,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>6</v>
       </c>
@@ -620,16 +635,51 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>42</v>
       </c>
       <c r="B23" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28">
+        <v>273</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;1#&amp;"Arial Black"&amp;10&amp;K4099DAINTERNAL</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Use same openpyxl.load_workbook() args as in pandas.read_excel(), notably data_only=True
</commit_message>
<xml_diff>
--- a/pdtable/test/io/input/foo.xlsx
+++ b/pdtable/test/io/input/foo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeaco\repos\pdtable\pdtable\test\io\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1221CD82-89E3-42F8-AFFA-77B254447387}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F42FE48-99BA-4A2F-890C-5C0D2630509D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0C2B564F-1ED4-41D9-860E-6D5D2FB64FA7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0C2B564F-1ED4-41D9-860E-6D5D2FB64FA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -75,9 +77,6 @@
     <t>one</t>
   </si>
   <si>
-    <t>six</t>
-  </si>
-  <si>
     <t>forty-two</t>
   </si>
   <si>
@@ -127,6 +126,9 @@
   </si>
   <si>
     <t>**this_one_is_transposed*</t>
+  </si>
+  <si>
+    <t>six, as formula</t>
   </si>
 </sst>
 </file>
@@ -480,54 +482,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B433973-3070-4A41-BCCD-AE6DD659FC75}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>22</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -538,7 +540,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -549,7 +551,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -560,7 +562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -571,7 +573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -582,7 +584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -590,28 +592,28 @@
         <v>11</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -619,7 +621,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
@@ -627,49 +629,50 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
+        <f>2*3</f>
         <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
         <v>27</v>
-      </c>
-      <c r="B27" t="s">
-        <v>28</v>
       </c>
       <c r="C27">
         <v>1.23</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
         <v>29</v>
-      </c>
-      <c r="B28" t="s">
-        <v>30</v>
       </c>
       <c r="C28">
         <v>273</v>

</xml_diff>